<commit_message>
update the app with download function
</commit_message>
<xml_diff>
--- a/script/darkzone.xlsx
+++ b/script/darkzone.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\Documents\GitHub\PhD\remote-sensing-of-albedo--development-\final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\Documents\GitHub\PhD\Remote-Sensing-of-Albedo\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BC1386-F43C-4580-9FC4-B5088CBDC1CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E58B093-7C6C-4823-8835-00CD9AB9A1B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{BCEFC0CC-C4F7-41E7-8231-B995CCB6EDF2}"/>
+    <workbookView xWindow="1830" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{BCEFC0CC-C4F7-41E7-8231-B995CCB6EDF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>1984-1990</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>min 78 m2 0.45</t>
+  </si>
+  <si>
+    <t>1984-2004</t>
+  </si>
+  <si>
+    <t>2005-2007</t>
+  </si>
+  <si>
+    <t>2008-2020</t>
+  </si>
+  <si>
+    <t>km2 mean</t>
   </si>
 </sst>
 </file>
@@ -101,10 +113,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,15 +1098,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1418,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E33AB18-87D3-4960-97B4-A9BE74B586AD}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1442,7 @@
     <col min="2" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1442,8 +1455,11 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1457,8 +1473,15 @@
         <f>B2/1000000</f>
         <v>3443.1586240086099</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(D2:D8)</f>
+        <v>3609.150001043995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1472,8 +1495,15 @@
         <f t="shared" ref="D3:D24" si="0">B3/1000000</f>
         <v>3857.7725835691399</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <f>AVERAGE(D9:D11)</f>
+        <v>7598.6297977734939</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1487,8 +1517,19 @@
         <f t="shared" si="0"/>
         <v>5464.1764516427302</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <f>AVERAGE(D12:D24)</f>
+        <v>8358.8698049071118</v>
+      </c>
+      <c r="I4" s="3">
+        <f>(H4-H2)/H2</f>
+        <v>1.3160217232559457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -1503,7 +1544,7 @@
         <v>4041.57648267691</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2002</v>
       </c>
@@ -1518,7 +1559,7 @@
         <v>2728.7974041048697</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2003</v>
       </c>
@@ -1533,7 +1574,7 @@
         <v>3137.7864817627801</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2004</v>
       </c>
@@ -1548,7 +1589,7 @@
         <v>2590.78197954292</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2005</v>
       </c>
@@ -1563,7 +1604,7 @@
         <v>6185.72153892805</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2006</v>
       </c>
@@ -1578,7 +1619,7 @@
         <v>6093.7055238275298</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>
@@ -1593,7 +1634,7 @@
         <v>10516.4623305649</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2008</v>
       </c>
@@ -1608,7 +1649,7 @@
         <v>9046.1153131501196</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2009</v>
       </c>
@@ -1623,7 +1664,7 @@
         <v>7353.2984851769106</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
@@ -1638,7 +1679,7 @@
         <v>11798.468458015401</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -1653,7 +1694,7 @@
         <v>6566.1305005795293</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>

</xml_diff>

<commit_message>
clean up before submitting
</commit_message>
<xml_diff>
--- a/script/darkzone.xlsx
+++ b/script/darkzone.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\Documents\GitHub\PhD\Remote-Sensing-of-Albedo\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E58B093-7C6C-4823-8835-00CD9AB9A1B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD48F7C1-E7F3-4F69-A665-126AFE0CABF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{BCEFC0CC-C4F7-41E7-8231-B995CCB6EDF2}"/>
+    <workbookView xWindow="1704" yWindow="732" windowWidth="27000" windowHeight="13224" xr2:uid="{BCEFC0CC-C4F7-41E7-8231-B995CCB6EDF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>1984-1990</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>km2</t>
-  </si>
-  <si>
-    <t>min78 m2</t>
   </si>
   <si>
     <t>min 78 m2 0.45</t>
@@ -113,10 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -190,7 +186,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -290,78 +286,78 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$24</c:f>
+              <c:f>Sheet1!$C$2:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>3443.1586240086099</c:v>
+                  <c:v>2982.2753368035596</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3857.7725835691399</c:v>
+                  <c:v>3342.5352262813603</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5464.1764516427302</c:v>
+                  <c:v>5276.6717354082402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4041.57648267691</c:v>
+                  <c:v>3912.8477460925001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2728.7974041048697</c:v>
+                  <c:v>2614.7317225745701</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3137.7864817627801</c:v>
+                  <c:v>3032.72776838963</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2590.78197954292</c:v>
+                  <c:v>2486.2221671809502</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6185.72153892805</c:v>
+                  <c:v>6131.4228419177307</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6093.7055238275298</c:v>
+                  <c:v>5975.4336713672401</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10516.4623305649</c:v>
+                  <c:v>10485.177827728201</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9046.1153131501196</c:v>
+                  <c:v>8956.5786561823006</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7353.2984851769106</c:v>
+                  <c:v>7212.6387399220803</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11798.468458015401</c:v>
+                  <c:v>11804.0689167947</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6566.1305005795293</c:v>
+                  <c:v>6444.0224186795194</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10562.9617542345</c:v>
+                  <c:v>10446.949205181199</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7121.7703326413903</c:v>
+                  <c:v>7006.3350601411694</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10096.183462856101</c:v>
+                  <c:v>10029.9076549085</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3276.9314277333597</c:v>
+                  <c:v>3183.7028028784298</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10163.1056301723</c:v>
+                  <c:v>10196.072328743099</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8500.98388319689</c:v>
+                  <c:v>8495.7929170384305</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6107.5954610511908</c:v>
+                  <c:v>6015.1315869759201</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11036.440723158899</c:v>
+                  <c:v>11034.799341075301</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7035.32203182587</c:v>
+                  <c:v>6988.3254077599095</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1097,16 +1093,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>542924</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>497204</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1431,402 +1427,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E33AB18-87D3-4960-97B4-A9BE74B586AD}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E21"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>3443158624.0086098</v>
-      </c>
-      <c r="C2" s="2">
-        <v>4095118207.08042</v>
-      </c>
-      <c r="D2">
+        <v>2982275336.8035598</v>
+      </c>
+      <c r="C2">
         <f>B2/1000000</f>
-        <v>3443.1586240086099</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <f>AVERAGE(D2:D8)</f>
-        <v>3609.150001043995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2982.2753368035596</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(C2:C8)</f>
+        <v>3378.2873861044018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>3857772583.56914</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5223245874.1345701</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D24" si="0">B3/1000000</f>
-        <v>3857.7725835691399</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <f>AVERAGE(D9:D11)</f>
-        <v>7598.6297977734939</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3342535226.2813601</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C24" si="0">B3/1000000</f>
+        <v>3342.5352262813603</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <f>AVERAGE(C9:C11)</f>
+        <v>7530.678113671057</v>
+      </c>
+      <c r="H3" s="2">
+        <f>(G3-G2)/G2</f>
+        <v>1.2291407606843341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>5464176451.6427298</v>
-      </c>
-      <c r="C4" s="1">
-        <v>10800697677.406601</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>5464.1764516427302</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <f>AVERAGE(D12:D24)</f>
-        <v>8358.8698049071118</v>
-      </c>
-      <c r="I4" s="3">
-        <f>(H4-H2)/H2</f>
-        <v>1.3160217232559457</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5276671735.4082403</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>5276.6717354082402</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <f>AVERAGE(C12:C24)</f>
+        <v>8293.4096181754267</v>
+      </c>
+      <c r="H4" s="2">
+        <f>(G4-G2)/G2</f>
+        <v>1.4549153669660977</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2001</v>
       </c>
       <c r="B5" s="1">
-        <v>4041576482.6769099</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9775111754.4701805</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>4041.57648267691</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3912847746.0925002</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3912.8477460925001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2002</v>
       </c>
       <c r="B6" s="1">
-        <v>2728797404.1048698</v>
-      </c>
-      <c r="C6" s="1">
-        <v>6157079684.89713</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>2728.7974041048697</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2614731722.5745702</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2614.7317225745701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2003</v>
       </c>
       <c r="B7" s="1">
-        <v>3137786481.7627802</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6406436366.9351997</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>3137.7864817627801</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3032727768.3896298</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3032.72776838963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2004</v>
       </c>
       <c r="B8" s="1">
-        <v>2590781979.5429201</v>
-      </c>
-      <c r="C8" s="1">
-        <v>6644767943.5259705</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>2590.78197954292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2486222167.1809502</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2486.2221671809502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2005</v>
       </c>
       <c r="B9" s="1">
-        <v>6185721538.92805</v>
-      </c>
-      <c r="C9" s="1">
-        <v>10228760849.808001</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>6185.72153892805</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6131422841.9177303</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>6131.4228419177307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2006</v>
       </c>
       <c r="B10" s="1">
-        <v>6093705523.8275299</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10262007010.7202</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>6093.7055238275298</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5975433671.36724</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5975.4336713672401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2007</v>
       </c>
       <c r="B11" s="1">
-        <v>10516462330.564899</v>
-      </c>
-      <c r="C11" s="1">
-        <v>15273425166.140699</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>10516.4623305649</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10485177827.728201</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>10485.177827728201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2008</v>
       </c>
       <c r="B12" s="1">
-        <v>9046115313.1501198</v>
-      </c>
-      <c r="C12" s="1">
-        <v>14102390045.794001</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>9046.1153131501196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>8956578656.1823006</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>8956.5786561823006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2009</v>
       </c>
       <c r="B13" s="1">
-        <v>7353298485.1769104</v>
-      </c>
-      <c r="C13" s="1">
-        <v>11725615633.2188</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>7353.2984851769106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>7212638739.92208</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>7212.6387399220803</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2010</v>
       </c>
       <c r="B14" s="1">
-        <v>11798468458.0154</v>
-      </c>
-      <c r="C14" s="1">
-        <v>16264849929.493999</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>11798.468458015401</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11804068916.794701</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>11804.0689167947</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2011</v>
       </c>
       <c r="B15" s="1">
-        <v>6566130500.5795298</v>
-      </c>
-      <c r="C15" s="1">
-        <v>12913356146.186001</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>6566.1305005795293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6444022418.6795197</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>6444.0224186795194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2012</v>
       </c>
       <c r="B16" s="1">
-        <v>10562961754.234501</v>
-      </c>
-      <c r="C16" s="1">
-        <v>16934934784.24</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>10562.9617542345</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10446949205.1812</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>10446.949205181199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2013</v>
       </c>
       <c r="B17" s="1">
-        <v>7121770332.6413898</v>
-      </c>
-      <c r="C17" s="1">
-        <v>13384552318.795</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>7121.7703326413903</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7006335060.1411695</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>7006.3350601411694</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2014</v>
       </c>
       <c r="B18" s="1">
-        <v>10096183462.8561</v>
-      </c>
-      <c r="C18" s="1">
-        <v>16342451951.4911</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>10096.183462856101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10029907654.908501</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>10029.9076549085</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2015</v>
       </c>
       <c r="B19" s="1">
-        <v>3276931427.7333598</v>
-      </c>
-      <c r="C19" s="1">
-        <v>8470014604.3934698</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>3276.9314277333597</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3183702802.8784299</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>3183.7028028784298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2016</v>
       </c>
       <c r="B20" s="1">
-        <v>10163105630.1723</v>
-      </c>
-      <c r="C20" s="1">
-        <v>16318755904.878099</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>10163.1056301723</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10196072328.743099</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>10196.072328743099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2017</v>
       </c>
       <c r="B21" s="1">
-        <v>8500983883.1968899</v>
-      </c>
-      <c r="C21" s="1">
-        <v>13265798917.5273</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>8500.98388319689</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8495792917.0384302</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>8495.7929170384305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2018</v>
       </c>
       <c r="B22" s="1">
-        <v>6107595461.0511904</v>
-      </c>
-      <c r="C22" s="1">
-        <v>11778160075.2055</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>6107.5954610511908</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6015131586.9759197</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>6015.1315869759201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
       <c r="B23" s="1">
-        <v>11036440723.158899</v>
-      </c>
-      <c r="C23" s="1">
-        <v>16827655519.3999</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>11036.440723158899</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11034799341.0753</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>11034.799341075301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2020</v>
       </c>
       <c r="B24" s="1">
-        <v>7035322031.8258696</v>
-      </c>
-      <c r="C24" s="1">
-        <v>12590989717.970501</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>7035.32203182587</v>
+        <v>6988325407.7599096</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>6988.3254077599095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>